<commit_message>
new data morning 0708/2024
</commit_message>
<xml_diff>
--- a/Draft/url.xlsx
+++ b/Draft/url.xlsx
@@ -27,9 +27,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926081452895196?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/903821068439059?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/903153778505788?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/902629631891536?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/902511645236668?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/902438565243976?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/902270611927438?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/902213735266459?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/902185381935961?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926752122828129?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926457522857589?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926382092865132?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926308382872503?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926251742878167?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926178166218858?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926045759565432?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/925408646295810?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/925780072925334?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/926976216139053?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -53,15 +110,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -515,12 +572,12 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -645,18 +702,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,13 +1240,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD60"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="16384" width="8.88888888888889" style="1"/>
   </cols>
@@ -1206,59 +1256,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:1">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:1">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:1">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:1">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:1">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:1">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:1">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:1">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:1">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="1:3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>